<commit_message>
Revert "Updated product Status"
This reverts commit 723b6c5f72226c25cc457578a32c78e3b4ccfd9e.
</commit_message>
<xml_diff>
--- a/Project Overview.xlsx
+++ b/Project Overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Page</t>
   </si>
@@ -128,15 +128,6 @@
   </si>
   <si>
     <t>Tuesday, November 4</t>
-  </si>
-  <si>
-    <t>Add booking form (order page) to front page?</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>Jose</t>
   </si>
 </sst>
 </file>
@@ -514,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,9 +698,7 @@
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -851,9 +840,7 @@
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -908,9 +895,7 @@
     </row>
     <row r="31" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Updated Project Plan, Meeting Agenda
Added a meeting agenda and some deliverables to the project plan.
</commit_message>
<xml_diff>
--- a/Project Overview.xlsx
+++ b/Project Overview.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
-  <si>
-    <t>Page</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>Tasks (Phase 1) : HTML/CSS/JS</t>
   </si>
@@ -28,9 +25,6 @@
     <t>People Responsible</t>
   </si>
   <si>
-    <t>Deadline</t>
-  </si>
-  <si>
     <t>Main (index.html) / General</t>
   </si>
   <si>
@@ -58,15 +52,9 @@
     <t>Update to generate the agency information from the database</t>
   </si>
   <si>
-    <t>Display information nicely</t>
-  </si>
-  <si>
     <t>Vacation Packages</t>
   </si>
   <si>
-    <t>Add PHP that grabs the packages from the database</t>
-  </si>
-  <si>
     <t>Display package information nicely</t>
   </si>
   <si>
@@ -79,12 +67,6 @@
     <t>Order page</t>
   </si>
   <si>
-    <t>Link to database</t>
-  </si>
-  <si>
-    <t>customer data booking record</t>
-  </si>
-  <si>
     <t>Extra features (ideas)</t>
   </si>
   <si>
@@ -94,40 +76,97 @@
     <t>In presentation talk about the technology</t>
   </si>
   <si>
-    <t>Modular design for easy CSS targeting (Done)</t>
-  </si>
-  <si>
-    <t>Change design (background image, colours) (Leisy)</t>
-  </si>
-  <si>
-    <t>Create a form for a customer to create an account (use JS) with their name, address, phone, userID, password. Data should go to bouncer,php. (Leisy)</t>
-  </si>
-  <si>
-    <t>Create static page with information about how to phone, email, or go to the agency (jose)</t>
-  </si>
-  <si>
-    <t>Create a “Vacation Package” page listing all vacation packages available. (static for now) (Darcie)</t>
-  </si>
-  <si>
-    <t>Darcie: Add DB to Git and commit</t>
-  </si>
-  <si>
-    <t>Import database and link to all pages that need it (Jasmeen)</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Responsive Design for Mobile</t>
   </si>
   <si>
-    <t>Link to Registration, packages, and contact  (Jasmeen)</t>
-  </si>
-  <si>
     <t>Date Completed</t>
   </si>
   <si>
     <t>Tuesday, November 4</t>
+  </si>
+  <si>
+    <t>Darcie</t>
+  </si>
+  <si>
+    <t>Friday November 7</t>
+  </si>
+  <si>
+    <t>Add PHP that grabs the valid packages from the database</t>
+  </si>
+  <si>
+    <t>Leisy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a form for a customer to create an account (use JS) with their name, address, phone, userID, password. Data should go to bouncer,php. </t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create static page with information about how to phone, email, or go to the agency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links to Registration, packages, and contact </t>
+  </si>
+  <si>
+    <t>Page / Feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an order page for customers to enter their information </t>
+  </si>
+  <si>
+    <t>Insert booking record into database</t>
+  </si>
+  <si>
+    <t>Display information nicely (edit CSS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Go through code and make sure everything has an author, consistent comment style, intenting, etc.</t>
+  </si>
+  <si>
+    <t>Leisy?</t>
+  </si>
+  <si>
+    <t>Create a “Vacation Package” page listing all vacation packages available. (static for now)</t>
+  </si>
+  <si>
+    <t>Presentation Lead(s)</t>
+  </si>
+  <si>
+    <t>Create plan for presentation</t>
+  </si>
+  <si>
+    <t>Create slides for presentation</t>
+  </si>
+  <si>
+    <t>Test all completed pages for functionality, completion of assignment requirements, and consistent professional look, feel, &amp; user experience</t>
+  </si>
+  <si>
+    <t>Export updated DB to Git and commit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import database and link to all pages that need it </t>
+  </si>
+  <si>
+    <t>Create page tenplates, modular design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change design (background image, colours) </t>
+  </si>
+  <si>
+    <t>Leisy and Jasmeen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front page booking form </t>
   </si>
 </sst>
 </file>
@@ -503,45 +542,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -550,40 +593,53 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -592,8 +648,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -602,26 +659,32 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -630,8 +693,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -640,24 +704,32 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -666,8 +738,9 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -676,8 +749,9 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -686,36 +760,47 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -724,8 +809,9 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -734,8 +820,9 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -744,62 +831,77 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -808,8 +910,9 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -818,8 +921,9 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -828,36 +932,47 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -866,8 +981,9 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -876,36 +992,41 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -914,8 +1035,9 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -924,6 +1046,110 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Packages page and updated database
Added the DB functionality to the packages page. Please import this new
database file because I updated the data to have current dates.
</commit_message>
<xml_diff>
--- a/Project Overview.xlsx
+++ b/Project Overview.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Tasks (Phase 1) : HTML/CSS/JS</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t xml:space="preserve">Front page booking form </t>
+  </si>
+  <si>
+    <t>Sunday November 9</t>
+  </si>
+  <si>
+    <t>having trouble reformatting the dates</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Added order button (Nov 10), but they have no function yet</t>
   </si>
 </sst>
 </file>
@@ -203,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -226,16 +238,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -545,7 +592,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H19" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +606,7 @@
     <col min="9" max="9" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -581,8 +628,10 @@
       <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1"/>
+      <c r="H1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -592,8 +641,8 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -615,8 +664,8 @@
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
@@ -636,8 +685,8 @@
         <v>24</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
@@ -647,8 +696,8 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
@@ -658,8 +707,8 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -681,8 +730,8 @@
         <v>7</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
@@ -692,8 +741,8 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
@@ -703,8 +752,8 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -726,8 +775,8 @@
         <v>27</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -737,10 +786,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -748,8 +797,8 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
@@ -759,8 +808,8 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -784,8 +833,8 @@
       <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
@@ -797,8 +846,8 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -808,8 +857,8 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
@@ -819,8 +868,8 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
@@ -830,8 +879,8 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -852,11 +901,13 @@
       <c r="F19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -867,9 +918,13 @@
       <c r="F20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
@@ -883,8 +938,8 @@
         <v>24</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
@@ -898,8 +953,10 @@
         <v>24</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="H22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -909,8 +966,8 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
@@ -920,8 +977,8 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
@@ -931,8 +988,8 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -954,8 +1011,8 @@
         <v>29</v>
       </c>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
@@ -969,8 +1026,8 @@
         <v>29</v>
       </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
@@ -980,8 +1037,8 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
@@ -991,8 +1048,8 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -1008,8 +1065,8 @@
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
@@ -1023,8 +1080,8 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
@@ -1034,8 +1091,8 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
@@ -1045,8 +1102,8 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
@@ -1056,8 +1113,8 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
@@ -1079,8 +1136,8 @@
         <v>37</v>
       </c>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
@@ -1094,8 +1151,8 @@
         <v>37</v>
       </c>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
@@ -1105,8 +1162,8 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
@@ -1122,8 +1179,8 @@
         <v>37</v>
       </c>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
@@ -1137,8 +1194,8 @@
         <v>37</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
@@ -1148,10 +1205,52 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Done the packages page
</commit_message>
<xml_diff>
--- a/Project Overview.xlsx
+++ b/Project Overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Tasks (Phase 1) : HTML/CSS/JS</t>
   </si>
@@ -624,7 +624,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -634,6 +636,7 @@
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="25.88671875" customWidth="1"/>
     <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
     <col min="9" max="9" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -959,7 +962,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -970,7 +973,9 @@
       <c r="F21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
     </row>
@@ -1272,26 +1277,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
@@ -1304,14 +1297,26 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to presentation plan
Added some items that need doing
</commit_message>
<xml_diff>
--- a/Project Overview.xlsx
+++ b/Project Overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Tasks (Phase 1) : HTML/CSS/JS</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Create a “Vacation Package” page listing all vacation packages available. (static for now)</t>
   </si>
   <si>
-    <t>Create plan for presentation</t>
-  </si>
-  <si>
     <t>Create slides for presentation</t>
   </si>
   <si>
@@ -209,6 +206,12 @@
   </si>
   <si>
     <t>Thursday November 13</t>
+  </si>
+  <si>
+    <t>Create plan for presentation (structure)</t>
+  </si>
+  <si>
+    <t>Sunday November 17</t>
   </si>
 </sst>
 </file>
@@ -627,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I1" s="6"/>
     </row>
@@ -692,16 +695,16 @@
         <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
@@ -709,22 +712,22 @@
     <row r="4" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
@@ -756,13 +759,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>6</v>
@@ -816,7 +819,7 @@
         <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
@@ -945,7 +948,7 @@
         <v>24</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="6"/>
@@ -962,7 +965,7 @@
         <v>24</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
@@ -979,7 +982,7 @@
         <v>24</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
@@ -997,7 +1000,7 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I22" s="6"/>
     </row>
@@ -1048,7 +1051,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>29</v>
@@ -1085,19 +1088,19 @@
     </row>
     <row r="29" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="6"/>
@@ -1135,7 +1138,7 @@
     <row r="32" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
@@ -1155,7 +1158,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>24</v>
@@ -1200,7 +1203,7 @@
         <v>20</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>4</v>
@@ -1218,7 +1221,7 @@
         <v>37</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="5"/>
@@ -1237,18 +1240,20 @@
     </row>
     <row r="39" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G39" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="H39" s="5"/>
       <c r="I39" s="6"/>
     </row>
@@ -1258,10 +1263,10 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="5"/>
@@ -1273,10 +1278,10 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="5"/>
@@ -1284,26 +1289,14 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
@@ -1316,14 +1309,26 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>